<commit_message>
Update README with detailed security topics
Expanded the README to specify which security problems will be researched for the GDC and which will be explored as extra topics. Added notes and organized the list of security issues for clarity.
</commit_message>
<xml_diff>
--- a/docs/Official/Logboek GDC.xlsx
+++ b/docs/Official/Logboek GDC.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\GDC-Ian-2025-2026\docs\Official\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="B:\GitHub\GDC-Ian-2025-2026\docs\Official\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18B4392E-FA59-4016-9BC5-BDCD0415DA1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B302B8D-7F9D-4D1D-82A0-24E179252516}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{436E9E8A-65C9-4475-9C60-C188DFBA05A4}"/>
+    <workbookView xWindow="-28920" yWindow="5175" windowWidth="29040" windowHeight="15720" xr2:uid="{436E9E8A-65C9-4475-9C60-C188DFBA05A4}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="46">
   <si>
     <t>Datum:</t>
   </si>
@@ -166,10 +166,25 @@
 JWT Token, bevat user info -&gt; base64 format, geen encryptie dus geen gevoelige data opslaan</t>
   </si>
   <si>
+    <t>Verschillende security probelemen die betrekking hebben met elkaar, gaan vergelijken.</t>
+  </si>
+  <si>
+    <t>Injection Flaws vs IDOR vs trusting client data</t>
+  </si>
+  <si>
+    <t>Van toepassing voor beveiliging van XSS &amp; CSRF</t>
+  </si>
+  <si>
+    <t>XSS in detail</t>
+  </si>
+  <si>
+    <t>CSRF in detail</t>
+  </si>
+  <si>
     <t>V - XSS - Cross-Site Scripting, zeker bespreken
 V - CSRF - Cross-Site Request Forgery, zeker bespreken
 M - Injection Flaws (SQL, cmd, query), misschien bespreken
-X BOLA (Broken Object Level Authorization), niet bespreken
+X - BOLA (Broken Object Level Authorization), niet bespreken
 X - DDoS attacks, niet bespreken
 EX - Lack of  Rate Limiting, niet bespreken, wel extra onderzoeken
 X - Broken Authentication, niet bespreken
@@ -178,15 +193,6 @@
 EX - Insufficient Logging &amp; Monitoring (malicious activities go unnoticed), niet bespreken, wel extra onderzoeken
 M - Excessive Data Exposure (data meegeven die onnodig is), misschien bespreken
 M - trusting (manipulated) client-side data, misschien bespreken</t>
-  </si>
-  <si>
-    <t>Verschillende security probelemen die betrekking hebben met elkaar, gaan vergelijken.</t>
-  </si>
-  <si>
-    <t>Injection Flaws vs IDOR vs trusting client data</t>
-  </si>
-  <si>
-    <t>Van toepassing voor beveiliging van XSS &amp; CSRF</t>
   </si>
 </sst>
 </file>
@@ -643,27 +649,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B59746C-283F-4A2C-85E0-EFA8BF3CE917}">
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="38.33203125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="10.5546875" style="5" customWidth="1"/>
-    <col min="3" max="3" width="8.5546875" style="7" customWidth="1"/>
-    <col min="4" max="4" width="70.109375" style="9" customWidth="1"/>
-    <col min="5" max="5" width="88.5546875" style="13" customWidth="1"/>
-    <col min="6" max="6" width="21.44140625" style="16" customWidth="1"/>
-    <col min="7" max="7" width="17.5546875" style="13" customWidth="1"/>
-    <col min="8" max="8" width="15.6640625" style="13" customWidth="1"/>
-    <col min="9" max="9" width="18.6640625" style="13" customWidth="1"/>
-    <col min="10" max="10" width="23.44140625" style="13" customWidth="1"/>
+    <col min="1" max="1" width="43.140625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="8.5703125" style="7" customWidth="1"/>
+    <col min="4" max="4" width="78.42578125" style="9" customWidth="1"/>
+    <col min="5" max="5" width="88.5703125" style="13" customWidth="1"/>
+    <col min="6" max="6" width="21.42578125" style="16" customWidth="1"/>
+    <col min="7" max="7" width="17.5703125" style="13" customWidth="1"/>
+    <col min="8" max="8" width="15.7109375" style="13" customWidth="1"/>
+    <col min="9" max="9" width="18.7109375" style="13" customWidth="1"/>
+    <col min="10" max="10" width="23.42578125" style="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
@@ -695,7 +701,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="177.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="177.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
@@ -709,7 +715,7 @@
         <v>5</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="F2" s="14" t="s">
         <v>6</v>
@@ -724,7 +730,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>11</v>
       </c>
@@ -738,7 +744,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>14</v>
       </c>
@@ -758,7 +764,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" ht="40.5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>20</v>
       </c>
@@ -790,7 +796,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>22</v>
       </c>
@@ -819,7 +825,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="87.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" ht="87.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>33</v>
       </c>
@@ -839,20 +845,30 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>36</v>
       </c>
       <c r="D9" s="9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
         <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
aanvulling lijst keuze security problemen
</commit_message>
<xml_diff>
--- a/docs/Official/Logboek GDC.xlsx
+++ b/docs/Official/Logboek GDC.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="B:\GitHub\GDC-Ian-2025-2026\docs\Official\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B302B8D-7F9D-4D1D-82A0-24E179252516}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09277880-30BF-48D3-ACA1-EC3B5BD1F227}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="5175" windowWidth="29040" windowHeight="15720" xr2:uid="{436E9E8A-65C9-4475-9C60-C188DFBA05A4}"/>
   </bookViews>
@@ -652,7 +652,7 @@
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -848,6 +848,12 @@
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>41</v>
+      </c>
+      <c r="B8" s="5">
+        <v>45986</v>
+      </c>
+      <c r="C8" s="7">
+        <v>0.84444444444444444</v>
       </c>
       <c r="D8" s="9" t="s">
         <v>40</v>

</xml_diff>

<commit_message>
Update Logboek GDC.xlsx - extra onderwerpen
Replaces the previous version of the Logboek GDC.xlsx file with an updated version. Details of the changes are contained within the updated spreadsheet.
</commit_message>
<xml_diff>
--- a/docs/Official/Logboek GDC.xlsx
+++ b/docs/Official/Logboek GDC.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="B:\GitHub\GDC-Ian-2025-2026\docs\Official\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09277880-30BF-48D3-ACA1-EC3B5BD1F227}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DB330C2-67D9-4F9D-ADD1-7DCEAD5DFA89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="5175" windowWidth="29040" windowHeight="15720" xr2:uid="{436E9E8A-65C9-4475-9C60-C188DFBA05A4}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="61">
   <si>
     <t>Datum:</t>
   </si>
@@ -173,12 +173,6 @@
   </si>
   <si>
     <t>Van toepassing voor beveiliging van XSS &amp; CSRF</t>
-  </si>
-  <si>
-    <t>XSS in detail</t>
-  </si>
-  <si>
-    <t>CSRF in detail</t>
   </si>
   <si>
     <t>V - XSS - Cross-Site Scripting, zeker bespreken
@@ -193,6 +187,57 @@
 EX - Insufficient Logging &amp; Monitoring (malicious activities go unnoticed), niet bespreken, wel extra onderzoeken
 M - Excessive Data Exposure (data meegeven die onnodig is), misschien bespreken
 M - trusting (manipulated) client-side data, misschien bespreken</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=EoaDgUgS6QA</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=z4LhLJnmoZ0</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=PKgw0CLZIhE&amp;t=20s</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=m-0p2BFAZvI</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=ej2O4lOUzRc</t>
+  </si>
+  <si>
+    <t>https://portswigger.net/web-security/cross-site-scripting</t>
+  </si>
+  <si>
+    <t>https://owasp.org/www-community/attacks/xss/</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/Cross-site_scripting</t>
+  </si>
+  <si>
+    <t>https://developer.mozilla.org/en-US/docs/Web/Security/Attacks/XSS</t>
+  </si>
+  <si>
+    <t>https://www.geeksforgeeks.org/ethical-hacking/what-is-cross-site-scripting-xss/</t>
+  </si>
+  <si>
+    <t>https://www.cloudflare.com/learning/security/threats/cross-site-scripting/</t>
+  </si>
+  <si>
+    <t>XSS Specifiek bij API's</t>
+  </si>
+  <si>
+    <t>CSP header</t>
+  </si>
+  <si>
+    <t>3 verschillende soorten XSS</t>
+  </si>
+  <si>
+    <t>XSS algemeen in detail</t>
+  </si>
+  <si>
+    <t>CSRF algemeen in detail</t>
+  </si>
+  <si>
+    <t>CSRF Spefifiek bij API's</t>
   </si>
 </sst>
 </file>
@@ -263,7 +308,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -314,6 +359,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -649,10 +695,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B59746C-283F-4A2C-85E0-EFA8BF3CE917}">
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:S14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -667,9 +713,10 @@
     <col min="8" max="8" width="15.7109375" style="13" customWidth="1"/>
     <col min="9" max="9" width="18.7109375" style="13" customWidth="1"/>
     <col min="10" max="10" width="23.42578125" style="13" customWidth="1"/>
+    <col min="11" max="19" width="23.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
@@ -700,8 +747,35 @@
       <c r="J1" s="8" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" ht="177.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K1" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="L1" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="M1" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="N1" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q1" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="R1" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="S1" s="8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" ht="177.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
@@ -715,7 +789,7 @@
         <v>5</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F2" s="14" t="s">
         <v>6</v>
@@ -730,7 +804,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>11</v>
       </c>
@@ -744,7 +818,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>14</v>
       </c>
@@ -764,7 +838,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="40.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" ht="40.5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>20</v>
       </c>
@@ -796,7 +870,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>22</v>
       </c>
@@ -825,7 +899,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="87.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" ht="87.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>33</v>
       </c>
@@ -845,7 +919,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>41</v>
       </c>
@@ -859,22 +933,90 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B9" s="5">
+        <v>46010</v>
+      </c>
+      <c r="C9" s="7">
+        <v>0.60763888888888884</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="F9" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="G9" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="H9" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="I9" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="J9" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="K9" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="L9" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="M9" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="N9" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="O9" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="P9" s="18" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D9" s="9" t="s">
+      <c r="D11" s="9" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>44</v>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F12" s="17"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="11"/>
+      <c r="J12" s="11"/>
+      <c r="K12" s="18"/>
+      <c r="L12" s="18"/>
+      <c r="M12" s="18"/>
+      <c r="N12" s="18"/>
+      <c r="O12" s="18"/>
+      <c r="P12" s="18"/>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -896,8 +1038,19 @@
     <hyperlink ref="I6" r:id="rId15" xr:uid="{71631EA3-09D0-4D5A-82FA-58219DE802F9}"/>
     <hyperlink ref="F7" r:id="rId16" xr:uid="{A8179F7F-A0B4-4264-A2DC-15B44AEF929A}"/>
     <hyperlink ref="J5" r:id="rId17" xr:uid="{F2854C7E-F7A3-4D1B-ACAA-14B7C586B7EF}"/>
+    <hyperlink ref="F9" r:id="rId18" xr:uid="{98ED6B34-E655-415C-9BA4-3159DB7C9664}"/>
+    <hyperlink ref="G9" r:id="rId19" xr:uid="{5442341A-5781-4177-8C1D-61064B8BD40D}"/>
+    <hyperlink ref="H9" r:id="rId20" xr:uid="{4F1122E6-5460-4865-A5D6-68B0238E1859}"/>
+    <hyperlink ref="I9" r:id="rId21" xr:uid="{A14507CB-0B09-43EB-B80F-41BD41F2F480}"/>
+    <hyperlink ref="J9" r:id="rId22" xr:uid="{1F70A6CF-BB55-469B-B72C-89906F5DD2CC}"/>
+    <hyperlink ref="K9" r:id="rId23" xr:uid="{EB7F5E85-1714-4C77-9A35-62147343D936}"/>
+    <hyperlink ref="L9" r:id="rId24" xr:uid="{EA7DB39A-64E5-4B5E-802B-AD32AF5ACF95}"/>
+    <hyperlink ref="M9" r:id="rId25" xr:uid="{C80DCA23-7CDE-4FAF-AFF3-F5287FD262F9}"/>
+    <hyperlink ref="N9" r:id="rId26" xr:uid="{F6784396-0A11-4D49-862B-0AF3D3AC9BF5}"/>
+    <hyperlink ref="O9" r:id="rId27" xr:uid="{57DA929D-ECFB-415B-838B-1FAE7F8360F1}"/>
+    <hyperlink ref="P9" r:id="rId28" xr:uid="{CBCFED1F-49D4-46D7-945D-9B81BDF21811}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId18"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId29"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Toevoegen CORS aan logboek
</commit_message>
<xml_diff>
--- a/docs/Official/Logboek GDC.xlsx
+++ b/docs/Official/Logboek GDC.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="B:\GitHub\GDC-Ian-2025-2026\docs\Official\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5E77058-FB90-4440-9EB7-23BEF84C436D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68803F7D-ACFB-4B39-8806-A7DFCBD54B34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="7770" windowWidth="28800" windowHeight="15390" xr2:uid="{436E9E8A-65C9-4475-9C60-C188DFBA05A4}"/>
+    <workbookView xWindow="38280" yWindow="7560" windowWidth="29040" windowHeight="15720" xr2:uid="{436E9E8A-65C9-4475-9C60-C188DFBA05A4}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="63">
   <si>
     <t>Datum:</t>
   </si>
@@ -241,6 +241,9 @@
   </si>
   <si>
     <t>zie GDC</t>
+  </si>
+  <si>
+    <t>CORS</t>
   </si>
 </sst>
 </file>
@@ -698,10 +701,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B59746C-283F-4A2C-85E0-EFA8BF3CE917}">
-  <dimension ref="A1:S14"/>
+  <dimension ref="A1:S15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -999,35 +1002,46 @@
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D11" s="9" t="s">
-        <v>42</v>
+        <v>62</v>
+      </c>
+      <c r="B11" s="5">
+        <v>46018</v>
+      </c>
+      <c r="C11" s="7">
+        <v>0.9375</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="F12" s="17"/>
-      <c r="G12" s="11"/>
-      <c r="H12" s="11"/>
-      <c r="I12" s="11"/>
-      <c r="J12" s="11"/>
-      <c r="K12" s="18"/>
-      <c r="L12" s="18"/>
-      <c r="M12" s="18"/>
-      <c r="N12" s="18"/>
-      <c r="O12" s="18"/>
-      <c r="P12" s="18"/>
+        <v>36</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>55</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="F13" s="17"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="11"/>
+      <c r="I13" s="11"/>
+      <c r="J13" s="11"/>
+      <c r="K13" s="18"/>
+      <c r="L13" s="18"/>
+      <c r="M13" s="18"/>
+      <c r="N13" s="18"/>
+      <c r="O13" s="18"/>
+      <c r="P13" s="18"/>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
         <v>60</v>
       </c>
     </row>

</xml_diff>

<commit_message>
HTTP Header Onderzoek Logboek Update
</commit_message>
<xml_diff>
--- a/docs/Official/Logboek GDC.xlsx
+++ b/docs/Official/Logboek GDC.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="B:\GitHub\GDC-Ian-2025-2026\docs\Official\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68803F7D-ACFB-4B39-8806-A7DFCBD54B34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD0BDB72-159A-42DE-8B8B-803482BE0F9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="7560" windowWidth="29040" windowHeight="15720" xr2:uid="{436E9E8A-65C9-4475-9C60-C188DFBA05A4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{436E9E8A-65C9-4475-9C60-C188DFBA05A4}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="66">
   <si>
     <t>Datum:</t>
   </si>
@@ -145,9 +145,6 @@
   </si>
   <si>
     <t>https://www.youtube.com/watch?v=vTroMvQy6K0</t>
-  </si>
-  <si>
-    <t>HSTS (HTTP Strict Transport Security)</t>
   </si>
   <si>
     <t>token in local storage -&gt; elke JS script kan aan die storage &amp; token
@@ -170,9 +167,6 @@
   </si>
   <si>
     <t>Injection Flaws vs IDOR vs trusting client data</t>
-  </si>
-  <si>
-    <t>Van toepassing voor beveiliging van XSS &amp; CSRF</t>
   </si>
   <si>
     <t>V - XSS - Cross-Site Scripting, zeker bespreken
@@ -222,12 +216,6 @@
     <t>https://www.cloudflare.com/learning/security/threats/cross-site-scripting/</t>
   </si>
   <si>
-    <t>XSS Specifiek bij API's</t>
-  </si>
-  <si>
-    <t>CSP header</t>
-  </si>
-  <si>
     <t>3 verschillende soorten XSS</t>
   </si>
   <si>
@@ -237,13 +225,41 @@
     <t>CSRF algemeen in detail</t>
   </si>
   <si>
-    <t>CSRF Spefifiek bij API's</t>
-  </si>
-  <si>
     <t>zie GDC</t>
   </si>
   <si>
     <t>CORS</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=4bQeGUzHpOE</t>
+  </si>
+  <si>
+    <t>setting voor SOP</t>
+  </si>
+  <si>
+    <t>versturen van ongewenste verzoeken, omzijlt CORS wegens server-side actie en geen client-side actie</t>
+  </si>
+  <si>
+    <t>meegeven welke site wel toegang mag hebben tot api data, browser site beveiliging</t>
+  </si>
+  <si>
+    <t>kleine regels die server mee geeft aan de browser, hoe de data veilig moet verwerkt worden
+wat de browser wel en niet mag doen met de data 
+Van toepassing voor beveiliging van XSS &amp; CSRF &amp; API</t>
+  </si>
+  <si>
+    <t>HTTP Header Settings</t>
+  </si>
+  <si>
+    <t>CSP, whitelist voor het laden van scripts &amp; bestanden, lijst met welke zaken er vertrouwd mogen werken
+- enkel deze zaken inladen &amp; bepaalde tags blokkeren
+HSTS, communicatie over HTTPS verplichten ipv HTTP
+Content Type nosniff, prevent tegen MIME sniffing, luistern naar server niet raden door te sniffen
+Referrer Policy, extra opzoek werk doen, geeft geen extra tags mee als het cross origin is
+CORS, toestaan van cross origin request en limiteren</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=fFHl7psnvz0</t>
   </si>
 </sst>
 </file>
@@ -314,7 +330,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -366,6 +382,9 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -701,19 +720,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B59746C-283F-4A2C-85E0-EFA8BF3CE917}">
-  <dimension ref="A1:S15"/>
+  <dimension ref="A1:S13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="43.140625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="42.28515625" style="2" customWidth="1"/>
     <col min="2" max="2" width="10.5703125" style="5" customWidth="1"/>
     <col min="3" max="3" width="8.5703125" style="7" customWidth="1"/>
-    <col min="4" max="4" width="78.42578125" style="9" customWidth="1"/>
-    <col min="5" max="5" width="88.5703125" style="13" customWidth="1"/>
+    <col min="4" max="4" width="90.5703125" style="9" customWidth="1"/>
+    <col min="5" max="5" width="97.7109375" style="13" customWidth="1"/>
     <col min="6" max="6" width="21.42578125" style="16" customWidth="1"/>
     <col min="7" max="7" width="17.5703125" style="13" customWidth="1"/>
     <col min="8" max="8" width="15.7109375" style="13" customWidth="1"/>
@@ -795,7 +814,7 @@
         <v>5</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F2" s="14" t="s">
         <v>6</v>
@@ -858,7 +877,7 @@
         <v>21</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F5" s="14" t="s">
         <v>23</v>
@@ -873,7 +892,7 @@
         <v>28</v>
       </c>
       <c r="J5" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:19" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -919,7 +938,7 @@
         <v>34</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F7" s="17" t="s">
         <v>35</v>
@@ -927,7 +946,7 @@
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B8" s="5">
         <v>45986</v>
@@ -936,12 +955,12 @@
         <v>0.84444444444444444</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B9" s="5">
         <v>46010</v>
@@ -950,48 +969,48 @@
         <v>0.60763888888888884</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="E9" s="13" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="F9" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="G9" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="H9" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="G9" s="11" t="s">
+      <c r="I9" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="H9" s="11" t="s">
+      <c r="J9" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="I9" s="11" t="s">
+      <c r="K9" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="J9" s="11" t="s">
+      <c r="L9" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="K9" s="18" t="s">
+      <c r="M9" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="L9" s="18" t="s">
+      <c r="N9" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="M9" s="18" t="s">
+      <c r="O9" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="N9" s="18" t="s">
+      <c r="P9" s="18" t="s">
         <v>52</v>
-      </c>
-      <c r="O9" s="18" t="s">
-        <v>53</v>
-      </c>
-      <c r="P9" s="18" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B10" s="5">
         <v>46017</v>
@@ -999,10 +1018,16 @@
       <c r="C10" s="7">
         <v>0.625</v>
       </c>
+      <c r="D10" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="E10" s="13" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B11" s="5">
         <v>46018</v>
@@ -1010,19 +1035,37 @@
       <c r="C11" s="7">
         <v>0.9375</v>
       </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="D11" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="E11" s="13" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" ht="99.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D12" s="9" t="s">
-        <v>42</v>
+        <v>63</v>
+      </c>
+      <c r="B12" s="5">
+        <v>46019</v>
+      </c>
+      <c r="C12" s="7">
+        <v>0.64930555555555558</v>
+      </c>
+      <c r="D12" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="E12" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="F12" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="G12" s="11" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>56</v>
-      </c>
       <c r="F13" s="17"/>
       <c r="G13" s="11"/>
       <c r="H13" s="11"/>
@@ -1034,16 +1077,6 @@
       <c r="N13" s="18"/>
       <c r="O13" s="18"/>
       <c r="P13" s="18"/>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>60</v>
-      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1075,8 +1108,10 @@
     <hyperlink ref="N9" r:id="rId26" xr:uid="{F6784396-0A11-4D49-862B-0AF3D3AC9BF5}"/>
     <hyperlink ref="O9" r:id="rId27" xr:uid="{57DA929D-ECFB-415B-838B-1FAE7F8360F1}"/>
     <hyperlink ref="P9" r:id="rId28" xr:uid="{CBCFED1F-49D4-46D7-945D-9B81BDF21811}"/>
+    <hyperlink ref="G12" r:id="rId29" xr:uid="{FF9D4F01-3966-4BE6-ABF2-6EDC8A58A730}"/>
+    <hyperlink ref="F12" r:id="rId30" xr:uid="{1E46E5FD-FC9B-4AFE-9021-5686FCC59D07}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId29"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId31"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Korte Cookie Info, Logboek
</commit_message>
<xml_diff>
--- a/docs/Official/Logboek GDC.xlsx
+++ b/docs/Official/Logboek GDC.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="B:\GitHub\GDC-Ian-2025-2026\docs\Official\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD0BDB72-159A-42DE-8B8B-803482BE0F9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DD4A661-3773-4FCB-8C27-93176D28D05A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{436E9E8A-65C9-4475-9C60-C188DFBA05A4}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="68">
   <si>
     <t>Datum:</t>
   </si>
@@ -260,6 +260,14 @@
   </si>
   <si>
     <t>https://www.youtube.com/watch?v=fFHl7psnvz0</t>
+  </si>
+  <si>
+    <t>Cookies</t>
+  </si>
+  <si>
+    <t>httponly
+samesite &amp; Cross Site
+secure</t>
   </si>
 </sst>
 </file>
@@ -723,7 +731,7 @@
   <dimension ref="A1:S13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1065,7 +1073,13 @@
         <v>65</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" ht="69" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>67</v>
+      </c>
       <c r="F13" s="17"/>
       <c r="G13" s="11"/>
       <c r="H13" s="11"/>

</xml_diff>